<commit_message>
Fix the BLUE-Inbound, use the stop IDs verbatim from the spreadsheet, add script to update gtfs based on timetable spreadsheet
</commit_message>
<xml_diff>
--- a/input-data/Lagos timetables.xlsx
+++ b/input-data/Lagos timetables.xlsx
@@ -73,6 +73,9 @@
     <t>Mile 2</t>
   </si>
   <si>
+    <t>Inbound</t>
+  </si>
+  <si>
     <t>Alaba</t>
   </si>
   <si>
@@ -83,9 +86,6 @@
   </si>
   <si>
     <t>RED</t>
-  </si>
-  <si>
-    <t>Inbound</t>
   </si>
   <si>
     <t>Agbado</t>
@@ -1762,7 +1762,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -1776,22 +1776,22 @@
         <v>17</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>5</v>
@@ -3011,7 +3011,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -3026,7 +3026,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3289,7 +3289,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>

</xml_diff>

<commit_message>
Recalculate afternoon blue inbound stop times (the official timetable is invalid)
</commit_message>
<xml_diff>
--- a/input-data/Lagos timetables.xlsx
+++ b/input-data/Lagos timetables.xlsx
@@ -2636,7 +2636,8 @@
         <v>0.7069212962962963</v>
       </c>
       <c r="K30" s="4">
-        <v>0.5653703703703704</v>
+        <f>J30+(K29-J29)</f>
+        <v>0.7111458333</v>
       </c>
     </row>
     <row r="31">
@@ -2668,7 +2669,8 @@
         <v>0.7229050925925926</v>
       </c>
       <c r="K31" s="4">
-        <v>0.5848263888888889</v>
+        <f>J31+(K29-J29)</f>
+        <v>0.7271296296</v>
       </c>
     </row>
     <row r="32">
@@ -2700,7 +2702,8 @@
         <v>0.7388888888888889</v>
       </c>
       <c r="K32" s="4">
-        <v>0.6042824074074075</v>
+        <f>J32+(K31-J31)</f>
+        <v>0.7431134259</v>
       </c>
     </row>
     <row r="33">
@@ -2732,7 +2735,8 @@
         <v>0.7548726851851851</v>
       </c>
       <c r="K33" s="4">
-        <v>0.6237384259259259</v>
+        <f>J33+(K31-J31)</f>
+        <v>0.7590972222</v>
       </c>
     </row>
     <row r="34">
@@ -2764,7 +2768,8 @@
         <v>0.7708564814814814</v>
       </c>
       <c r="K34" s="4">
-        <v>0.6431944444444444</v>
+        <f>J34+(K33-J33)</f>
+        <v>0.7750810185</v>
       </c>
     </row>
     <row r="35">
@@ -2796,7 +2801,8 @@
         <v>0.7868402777777778</v>
       </c>
       <c r="K35" s="4">
-        <v>0.6626504629629629</v>
+        <f>J35+(K33-J33)</f>
+        <v>0.7910648148</v>
       </c>
     </row>
     <row r="36">
@@ -2828,7 +2834,8 @@
         <v>0.8028240740740741</v>
       </c>
       <c r="K36" s="4">
-        <v>0.6791782407407407</v>
+        <f>J36+(K35-J35)</f>
+        <v>0.8070486111</v>
       </c>
     </row>
     <row r="37">
@@ -2860,7 +2867,8 @@
         <v>0.8188078703703704</v>
       </c>
       <c r="K37" s="4">
-        <v>0.695162037037037</v>
+        <f>J37+(K35-J35)</f>
+        <v>0.8230324074</v>
       </c>
     </row>
     <row r="38">

</xml_diff>